<commit_message>
Added X Structures template
</commit_message>
<xml_diff>
--- a/External Beam Templates/Structure Templates/Template Spreadsheets/Specialty Templates.xlsx
+++ b/External Beam Templates/Structure Templates/Template Spreadsheets/Specialty Templates.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9303"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="210" yWindow="270" windowWidth="27030" windowHeight="9885" activeTab="4"/>
@@ -11,18 +11,19 @@
     <sheet name="Booleans" sheetId="2" r:id="rId2"/>
     <sheet name="Artifact" sheetId="4" r:id="rId3"/>
     <sheet name="Helper" sheetId="5" r:id="rId4"/>
-    <sheet name="PET" sheetId="6" r:id="rId5"/>
-    <sheet name="SBRT Control" sheetId="7" r:id="rId6"/>
+    <sheet name="XSTRUCTURES" sheetId="8" r:id="rId5"/>
+    <sheet name="PET" sheetId="6" r:id="rId6"/>
+    <sheet name="SBRT Control" sheetId="7" r:id="rId7"/>
   </sheets>
   <externalReferences>
-    <externalReference r:id="rId7"/>
+    <externalReference r:id="rId8"/>
   </externalReferences>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="447" uniqueCount="168">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="518" uniqueCount="187">
   <si>
     <t>Bolus X cm thickness</t>
   </si>
@@ -526,6 +527,63 @@
   </si>
   <si>
     <t>TemplateFileName</t>
+  </si>
+  <si>
+    <t>XSTRUCTURES</t>
+  </si>
+  <si>
+    <t>RO Resident Contouring</t>
+  </si>
+  <si>
+    <t>RO Resident Contouring  X1 to X6, xGTV, xCTV, xPTV</t>
+  </si>
+  <si>
+    <t>X1</t>
+  </si>
+  <si>
+    <t>X2</t>
+  </si>
+  <si>
+    <t>X3</t>
+  </si>
+  <si>
+    <t>X4</t>
+  </si>
+  <si>
+    <t>X5</t>
+  </si>
+  <si>
+    <t>X6</t>
+  </si>
+  <si>
+    <t>xGTV</t>
+  </si>
+  <si>
+    <t>xCTV</t>
+  </si>
+  <si>
+    <t>xPTV</t>
+  </si>
+  <si>
+    <t>RO Resident GTV</t>
+  </si>
+  <si>
+    <t>RO Resident CTV</t>
+  </si>
+  <si>
+    <t>RO Resident PTV</t>
+  </si>
+  <si>
+    <t>X_structure Template.xml</t>
+  </si>
+  <si>
+    <t>PTV</t>
+  </si>
+  <si>
+    <t>CTV</t>
+  </si>
+  <si>
+    <t>GTV</t>
   </si>
 </sst>
 </file>
@@ -1078,7 +1136,7 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Title 2" xfId="1"/>
   </cellStyles>
-  <dxfs count="68">
+  <dxfs count="79">
     <dxf>
       <font>
         <b val="0"/>
@@ -1465,6 +1523,225 @@
     </dxf>
     <dxf>
       <border outline="0">
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
         <top style="thin">
           <color auto="1"/>
         </top>
@@ -2501,7 +2778,7 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table357911152285" displayName="Table357911152285" ref="A2:B13" totalsRowShown="0" headerRowDxfId="67" headerRowBorderDxfId="66" tableBorderDxfId="65" totalsRowBorderDxfId="64">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table357911152285" displayName="Table357911152285" ref="A2:B13" totalsRowShown="0" headerRowDxfId="78" headerRowBorderDxfId="77" tableBorderDxfId="76" totalsRowBorderDxfId="75">
   <tableColumns count="2">
     <tableColumn id="1" name="Attribute"/>
     <tableColumn id="2" name="Value"/>
@@ -2511,6 +2788,27 @@
 </file>
 
 <file path=xl/tables/table10.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="6" name="Table581012167" displayName="Table581012167" ref="D2:F11" totalsRowShown="0" headerRowDxfId="28" headerRowBorderDxfId="27" tableBorderDxfId="26" totalsRowBorderDxfId="25">
+  <tableColumns count="3">
+    <tableColumn id="1" name="Structure" dataDxfId="24"/>
+    <tableColumn id="2" name="ID" dataDxfId="23"/>
+    <tableColumn id="3" name="Name" dataDxfId="22"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table11.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="11" name="Table35697175" displayName="Table35697175" ref="A2:B13" totalsRowShown="0" headerRowDxfId="21" headerRowBorderDxfId="20" tableBorderDxfId="19" totalsRowBorderDxfId="18">
+  <tableColumns count="2">
+    <tableColumn id="1" name="Attribute"/>
+    <tableColumn id="2" name="Value"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight11" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table12.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="12" name="Table5707276" displayName="Table5707276" ref="D2:F8" totalsRowShown="0" headerRowDxfId="17" headerRowBorderDxfId="16" tableBorderDxfId="15" totalsRowBorderDxfId="14">
   <sortState ref="D3:H61">
     <sortCondition ref="E3:E61"/>
@@ -2524,7 +2822,7 @@
 </table>
 </file>
 
-<file path=xl/tables/table11.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/tables/table13.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="13" name="Table351321" displayName="Table351321" ref="A2:B13" totalsRowShown="0" headerRowDxfId="10" headerRowBorderDxfId="9" tableBorderDxfId="8" totalsRowBorderDxfId="7">
   <tableColumns count="2">
     <tableColumn id="1" name="Attribute"/>
@@ -2534,7 +2832,7 @@
 </table>
 </file>
 
-<file path=xl/tables/table12.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/tables/table14.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="14" name="Table51426" displayName="Table51426" ref="D2:F11" totalsRowShown="0" headerRowDxfId="6" headerRowBorderDxfId="5" tableBorderDxfId="4" totalsRowBorderDxfId="3">
   <tableColumns count="3">
     <tableColumn id="1" name="Structure" dataDxfId="2"/>
@@ -2546,7 +2844,28 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table581012162386" displayName="Table581012162386" ref="D2:F14" totalsRowShown="0" headerRowDxfId="63" headerRowBorderDxfId="62" tableBorderDxfId="61" totalsRowBorderDxfId="60">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table581012162386" displayName="Table581012162386" ref="D2:F14" totalsRowShown="0" headerRowDxfId="74" headerRowBorderDxfId="73" tableBorderDxfId="72" totalsRowBorderDxfId="71">
+  <tableColumns count="3">
+    <tableColumn id="1" name="Structure" dataDxfId="70"/>
+    <tableColumn id="2" name="ID" dataDxfId="69"/>
+    <tableColumn id="7" name="Name" dataDxfId="68"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table35791115228587" displayName="Table35791115228587" ref="A2:B13" totalsRowShown="0" headerRowDxfId="67" headerRowBorderDxfId="66" tableBorderDxfId="65" totalsRowBorderDxfId="64">
+  <tableColumns count="2">
+    <tableColumn id="1" name="Attribute"/>
+    <tableColumn id="2" name="Value"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight11" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Table58101216238688" displayName="Table58101216238688" ref="D2:F9" totalsRowShown="0" headerRowDxfId="63" headerRowBorderDxfId="62" tableBorderDxfId="61" totalsRowBorderDxfId="60">
   <tableColumns count="3">
     <tableColumn id="1" name="Structure" dataDxfId="59"/>
     <tableColumn id="2" name="ID" dataDxfId="58"/>
@@ -2556,29 +2875,8 @@
 </table>
 </file>
 
-<file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table35791115228587" displayName="Table35791115228587" ref="A2:B13" totalsRowShown="0" headerRowDxfId="56" headerRowBorderDxfId="55" tableBorderDxfId="54" totalsRowBorderDxfId="53">
-  <tableColumns count="2">
-    <tableColumn id="1" name="Attribute"/>
-    <tableColumn id="2" name="Value"/>
-  </tableColumns>
-  <tableStyleInfo name="TableStyleLight11" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
-</table>
-</file>
-
-<file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Table58101216238688" displayName="Table58101216238688" ref="D2:F9" totalsRowShown="0" headerRowDxfId="52" headerRowBorderDxfId="51" tableBorderDxfId="50" totalsRowBorderDxfId="49">
-  <tableColumns count="3">
-    <tableColumn id="1" name="Structure" dataDxfId="48"/>
-    <tableColumn id="2" name="ID" dataDxfId="47"/>
-    <tableColumn id="7" name="Name" dataDxfId="46"/>
-  </tableColumns>
-  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
-</table>
-</file>
-
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="7" name="Table3579111522" displayName="Table3579111522" ref="A2:B13" totalsRowShown="0" headerRowDxfId="45" headerRowBorderDxfId="44" tableBorderDxfId="43" totalsRowBorderDxfId="42">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="7" name="Table3579111522" displayName="Table3579111522" ref="A2:B13" totalsRowShown="0" headerRowDxfId="56" headerRowBorderDxfId="55" tableBorderDxfId="54" totalsRowBorderDxfId="53">
   <tableColumns count="2">
     <tableColumn id="1" name="Attribute"/>
     <tableColumn id="2" name="Value"/>
@@ -2588,20 +2886,20 @@
 </file>
 
 <file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="8" name="Table5810121623" displayName="Table5810121623" ref="D2:H10" totalsRowShown="0" headerRowDxfId="41" headerRowBorderDxfId="40" tableBorderDxfId="39" totalsRowBorderDxfId="38">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="8" name="Table5810121623" displayName="Table5810121623" ref="D2:H10" totalsRowShown="0" headerRowDxfId="52" headerRowBorderDxfId="51" tableBorderDxfId="50" totalsRowBorderDxfId="49">
   <tableColumns count="5">
-    <tableColumn id="1" name="Structure" dataDxfId="37"/>
-    <tableColumn id="2" name="ID" dataDxfId="36"/>
-    <tableColumn id="7" name="Name" dataDxfId="35"/>
-    <tableColumn id="6" name="SearchCTLow" dataDxfId="34"/>
-    <tableColumn id="5" name="SearchCTHigh" dataDxfId="33"/>
+    <tableColumn id="1" name="Structure" dataDxfId="48"/>
+    <tableColumn id="2" name="ID" dataDxfId="47"/>
+    <tableColumn id="7" name="Name" dataDxfId="46"/>
+    <tableColumn id="6" name="SearchCTLow" dataDxfId="45"/>
+    <tableColumn id="5" name="SearchCTHigh" dataDxfId="44"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="9" name="Table35791115" displayName="Table35791115" ref="A2:B13" totalsRowShown="0" headerRowDxfId="32" headerRowBorderDxfId="31" tableBorderDxfId="30" totalsRowBorderDxfId="29">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="9" name="Table35791115" displayName="Table35791115" ref="A2:B13" totalsRowShown="0" headerRowDxfId="43" headerRowBorderDxfId="42" tableBorderDxfId="41" totalsRowBorderDxfId="40">
   <tableColumns count="2">
     <tableColumn id="1" name="Attribute"/>
     <tableColumn id="2" name="Value"/>
@@ -2611,18 +2909,18 @@
 </file>
 
 <file path=xl/tables/table8.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="10" name="Table58101216" displayName="Table58101216" ref="D2:F12" totalsRowShown="0" headerRowDxfId="28" headerRowBorderDxfId="27" tableBorderDxfId="26" totalsRowBorderDxfId="25">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="10" name="Table58101216" displayName="Table58101216" ref="D2:F12" totalsRowShown="0" headerRowDxfId="39" headerRowBorderDxfId="38" tableBorderDxfId="37" totalsRowBorderDxfId="36">
   <tableColumns count="3">
-    <tableColumn id="1" name="Structure" dataDxfId="24"/>
-    <tableColumn id="2" name="ID" dataDxfId="23"/>
-    <tableColumn id="3" name="Name" dataDxfId="22"/>
+    <tableColumn id="1" name="Structure" dataDxfId="35"/>
+    <tableColumn id="2" name="ID" dataDxfId="34"/>
+    <tableColumn id="3" name="Name" dataDxfId="33"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table9.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="11" name="Table35697175" displayName="Table35697175" ref="A2:B13" totalsRowShown="0" headerRowDxfId="21" headerRowBorderDxfId="20" tableBorderDxfId="19" totalsRowBorderDxfId="18">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="Table357911156" displayName="Table357911156" ref="A2:B13" totalsRowShown="0" headerRowDxfId="32" headerRowBorderDxfId="31" tableBorderDxfId="30" totalsRowBorderDxfId="29">
   <tableColumns count="2">
     <tableColumn id="1" name="Attribute"/>
     <tableColumn id="2" name="Value"/>
@@ -6107,6 +6405,749 @@
   <dimension ref="A1:S13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B9" sqref="B9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="18.28515625" style="52" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="47.7109375" style="52" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="5.42578125" style="52" customWidth="1"/>
+    <col min="4" max="4" width="10.28515625" style="52" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="5.5703125" style="52" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="22.5703125" style="52" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="6.7109375" style="52" customWidth="1"/>
+    <col min="8" max="8" width="11.85546875" style="52" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="6" style="52" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="19.7109375" style="52" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="21" style="52" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="9.7109375" style="52" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="13.28515625" style="52" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="15.140625" style="52" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="14.42578125" style="52" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="14.140625" style="52" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="15.42578125" style="52" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="14" style="52" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="14.42578125" style="52" bestFit="1" customWidth="1"/>
+    <col min="20" max="16384" width="9.140625" style="52"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:19" ht="21" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="55" t="s">
+        <v>168</v>
+      </c>
+      <c r="B1" s="55"/>
+      <c r="C1" s="34"/>
+      <c r="D1" s="55" t="s">
+        <v>58</v>
+      </c>
+      <c r="E1" s="55"/>
+      <c r="F1" s="55"/>
+      <c r="H1" s="53" t="s">
+        <v>57</v>
+      </c>
+      <c r="I1" s="56"/>
+      <c r="J1" s="56"/>
+      <c r="K1" s="54"/>
+      <c r="L1" s="53" t="s">
+        <v>56</v>
+      </c>
+      <c r="M1" s="56"/>
+      <c r="N1" s="33" t="s">
+        <v>55</v>
+      </c>
+      <c r="O1" s="53" t="s">
+        <v>54</v>
+      </c>
+      <c r="P1" s="56"/>
+      <c r="Q1" s="54"/>
+      <c r="R1" s="53" t="s">
+        <v>53</v>
+      </c>
+      <c r="S1" s="54"/>
+    </row>
+    <row r="2" spans="1:19" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A2" s="31" t="s">
+        <v>52</v>
+      </c>
+      <c r="B2" s="32" t="s">
+        <v>51</v>
+      </c>
+      <c r="C2" s="24"/>
+      <c r="D2" s="31" t="s">
+        <v>32</v>
+      </c>
+      <c r="E2" s="30" t="s">
+        <v>37</v>
+      </c>
+      <c r="F2" s="43" t="s">
+        <v>50</v>
+      </c>
+      <c r="H2" s="29" t="s">
+        <v>49</v>
+      </c>
+      <c r="I2" s="27" t="s">
+        <v>48</v>
+      </c>
+      <c r="J2" s="27" t="s">
+        <v>47</v>
+      </c>
+      <c r="K2" s="25" t="s">
+        <v>46</v>
+      </c>
+      <c r="L2" s="26" t="s">
+        <v>45</v>
+      </c>
+      <c r="M2" s="27" t="s">
+        <v>44</v>
+      </c>
+      <c r="N2" s="28" t="s">
+        <v>43</v>
+      </c>
+      <c r="O2" s="26" t="s">
+        <v>42</v>
+      </c>
+      <c r="P2" s="27" t="s">
+        <v>41</v>
+      </c>
+      <c r="Q2" s="25" t="s">
+        <v>40</v>
+      </c>
+      <c r="R2" s="26" t="s">
+        <v>39</v>
+      </c>
+      <c r="S2" s="25" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="3" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A3" s="52" t="s">
+        <v>158</v>
+      </c>
+      <c r="B3" s="52" t="s">
+        <v>168</v>
+      </c>
+      <c r="C3" s="24"/>
+      <c r="D3" s="23" t="s">
+        <v>103</v>
+      </c>
+      <c r="E3" s="22" t="s">
+        <v>171</v>
+      </c>
+      <c r="F3" s="42" t="s">
+        <v>169</v>
+      </c>
+      <c r="H3" s="21" t="str">
+        <f>VLOOKUP(D3,[1]!Dictionary[#All],3,FALSE)</f>
+        <v>Artifact</v>
+      </c>
+      <c r="I3" s="20">
+        <f>VLOOKUP(D3,[1]!Dictionary[#All],4,FALSE)</f>
+        <v>11296</v>
+      </c>
+      <c r="J3" s="20" t="str">
+        <f>VLOOKUP(D3,[1]!Dictionary[#All],5,FALSE)</f>
+        <v>RADLEX</v>
+      </c>
+      <c r="K3" s="19">
+        <f>VLOOKUP(D3,[1]!Dictionary[#All],6,FALSE)</f>
+        <v>3.8</v>
+      </c>
+      <c r="L3" s="18" t="str">
+        <f>VLOOKUP(D3,[1]!VolumeType[#All],2,FALSE)</f>
+        <v>Artifact</v>
+      </c>
+      <c r="M3" s="17" t="str">
+        <f>VLOOKUP(D3,[1]!VolumeType[#All],3,FALSE)</f>
+        <v>None</v>
+      </c>
+      <c r="N3" s="16" t="str">
+        <f>VLOOKUP(D3,[1]!Colors[#All],3,FALSE)</f>
+        <v>z RO Helper</v>
+      </c>
+      <c r="O3" s="14" t="str">
+        <f>IFERROR(VLOOKUP(D3,[1]!DVH_lines[#Data],2,FALSE),"")</f>
+        <v/>
+      </c>
+      <c r="P3" s="15" t="str">
+        <f>IFERROR(VLOOKUP(D3,[1]!DVH_lines[#Data],3,FALSE),"")</f>
+        <v/>
+      </c>
+      <c r="Q3" s="13" t="str">
+        <f>IFERROR(VLOOKUP(D3,[1]!DVH_lines[#Data],4,FALSE),"")</f>
+        <v/>
+      </c>
+      <c r="R3" s="14" t="str">
+        <f>IFERROR(VLOOKUP(D3,[1]!SearchCT[#Data],2,FALSE),"")</f>
+        <v/>
+      </c>
+      <c r="S3" s="13" t="str">
+        <f>IFERROR(VLOOKUP(D3,[1]!SearchCT[#Data],3,FALSE),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="4" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A4" s="52" t="s">
+        <v>165</v>
+      </c>
+      <c r="B4" s="52" t="s">
+        <v>32</v>
+      </c>
+      <c r="C4" s="24"/>
+      <c r="D4" s="12" t="s">
+        <v>103</v>
+      </c>
+      <c r="E4" s="22" t="s">
+        <v>172</v>
+      </c>
+      <c r="F4" s="42" t="s">
+        <v>169</v>
+      </c>
+      <c r="H4" s="21" t="str">
+        <f>VLOOKUP(D4,[1]!Dictionary[#All],3,FALSE)</f>
+        <v>Artifact</v>
+      </c>
+      <c r="I4" s="20">
+        <f>VLOOKUP(D4,[1]!Dictionary[#All],4,FALSE)</f>
+        <v>11296</v>
+      </c>
+      <c r="J4" s="20" t="str">
+        <f>VLOOKUP(D4,[1]!Dictionary[#All],5,FALSE)</f>
+        <v>RADLEX</v>
+      </c>
+      <c r="K4" s="19">
+        <f>VLOOKUP(D4,[1]!Dictionary[#All],6,FALSE)</f>
+        <v>3.8</v>
+      </c>
+      <c r="L4" s="18" t="str">
+        <f>VLOOKUP(D4,[1]!VolumeType[#All],2,FALSE)</f>
+        <v>Artifact</v>
+      </c>
+      <c r="M4" s="17" t="str">
+        <f>VLOOKUP(D4,[1]!VolumeType[#All],3,FALSE)</f>
+        <v>None</v>
+      </c>
+      <c r="N4" s="16" t="str">
+        <f>VLOOKUP(D4,[1]!Colors[#All],3,FALSE)</f>
+        <v>z RO Helper</v>
+      </c>
+      <c r="O4" s="14" t="str">
+        <f>IFERROR(VLOOKUP(D4,[1]!DVH_lines[#Data],2,FALSE),"")</f>
+        <v/>
+      </c>
+      <c r="P4" s="15" t="str">
+        <f>IFERROR(VLOOKUP(D4,[1]!DVH_lines[#Data],3,FALSE),"")</f>
+        <v/>
+      </c>
+      <c r="Q4" s="13" t="str">
+        <f>IFERROR(VLOOKUP(D4,[1]!DVH_lines[#Data],4,FALSE),"")</f>
+        <v/>
+      </c>
+      <c r="R4" s="14" t="str">
+        <f>IFERROR(VLOOKUP(D4,[1]!SearchCT[#Data],2,FALSE),"")</f>
+        <v/>
+      </c>
+      <c r="S4" s="13" t="str">
+        <f>IFERROR(VLOOKUP(D4,[1]!SearchCT[#Data],3,FALSE),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="5" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A5" s="52" t="s">
+        <v>29</v>
+      </c>
+      <c r="B5" s="52" t="s">
+        <v>170</v>
+      </c>
+      <c r="C5" s="24"/>
+      <c r="D5" s="12" t="s">
+        <v>103</v>
+      </c>
+      <c r="E5" s="22" t="s">
+        <v>173</v>
+      </c>
+      <c r="F5" s="11" t="s">
+        <v>169</v>
+      </c>
+      <c r="H5" s="21" t="str">
+        <f>VLOOKUP(D5,[1]!Dictionary[#All],3,FALSE)</f>
+        <v>Artifact</v>
+      </c>
+      <c r="I5" s="20">
+        <f>VLOOKUP(D5,[1]!Dictionary[#All],4,FALSE)</f>
+        <v>11296</v>
+      </c>
+      <c r="J5" s="20" t="str">
+        <f>VLOOKUP(D5,[1]!Dictionary[#All],5,FALSE)</f>
+        <v>RADLEX</v>
+      </c>
+      <c r="K5" s="19">
+        <f>VLOOKUP(D5,[1]!Dictionary[#All],6,FALSE)</f>
+        <v>3.8</v>
+      </c>
+      <c r="L5" s="18" t="str">
+        <f>VLOOKUP(D5,[1]!VolumeType[#All],2,FALSE)</f>
+        <v>Artifact</v>
+      </c>
+      <c r="M5" s="17" t="str">
+        <f>VLOOKUP(D5,[1]!VolumeType[#All],3,FALSE)</f>
+        <v>None</v>
+      </c>
+      <c r="N5" s="16" t="str">
+        <f>VLOOKUP(D5,[1]!Colors[#All],3,FALSE)</f>
+        <v>z RO Helper</v>
+      </c>
+      <c r="O5" s="14" t="str">
+        <f>IFERROR(VLOOKUP(D5,[1]!DVH_lines[#Data],2,FALSE),"")</f>
+        <v/>
+      </c>
+      <c r="P5" s="15" t="str">
+        <f>IFERROR(VLOOKUP(D5,[1]!DVH_lines[#Data],3,FALSE),"")</f>
+        <v/>
+      </c>
+      <c r="Q5" s="13" t="str">
+        <f>IFERROR(VLOOKUP(D5,[1]!DVH_lines[#Data],4,FALSE),"")</f>
+        <v/>
+      </c>
+      <c r="R5" s="14" t="str">
+        <f>IFERROR(VLOOKUP(D5,[1]!SearchCT[#Data],2,FALSE),"")</f>
+        <v/>
+      </c>
+      <c r="S5" s="13" t="str">
+        <f>IFERROR(VLOOKUP(D5,[1]!SearchCT[#Data],3,FALSE),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="6" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A6" s="52" t="s">
+        <v>149</v>
+      </c>
+      <c r="B6" s="52">
+        <v>3</v>
+      </c>
+      <c r="C6" s="24"/>
+      <c r="D6" s="12" t="s">
+        <v>103</v>
+      </c>
+      <c r="E6" s="22" t="s">
+        <v>174</v>
+      </c>
+      <c r="F6" s="11" t="s">
+        <v>169</v>
+      </c>
+      <c r="H6" s="21" t="str">
+        <f>VLOOKUP(D6,[1]!Dictionary[#All],3,FALSE)</f>
+        <v>Artifact</v>
+      </c>
+      <c r="I6" s="20">
+        <f>VLOOKUP(D6,[1]!Dictionary[#All],4,FALSE)</f>
+        <v>11296</v>
+      </c>
+      <c r="J6" s="20" t="str">
+        <f>VLOOKUP(D6,[1]!Dictionary[#All],5,FALSE)</f>
+        <v>RADLEX</v>
+      </c>
+      <c r="K6" s="19">
+        <f>VLOOKUP(D6,[1]!Dictionary[#All],6,FALSE)</f>
+        <v>3.8</v>
+      </c>
+      <c r="L6" s="18" t="str">
+        <f>VLOOKUP(D6,[1]!VolumeType[#All],2,FALSE)</f>
+        <v>Artifact</v>
+      </c>
+      <c r="M6" s="17" t="str">
+        <f>VLOOKUP(D6,[1]!VolumeType[#All],3,FALSE)</f>
+        <v>None</v>
+      </c>
+      <c r="N6" s="16" t="str">
+        <f>VLOOKUP(D6,[1]!Colors[#All],3,FALSE)</f>
+        <v>z RO Helper</v>
+      </c>
+      <c r="O6" s="14" t="str">
+        <f>IFERROR(VLOOKUP(D6,[1]!DVH_lines[#Data],2,FALSE),"")</f>
+        <v/>
+      </c>
+      <c r="P6" s="15" t="str">
+        <f>IFERROR(VLOOKUP(D6,[1]!DVH_lines[#Data],3,FALSE),"")</f>
+        <v/>
+      </c>
+      <c r="Q6" s="13" t="str">
+        <f>IFERROR(VLOOKUP(D6,[1]!DVH_lines[#Data],4,FALSE),"")</f>
+        <v/>
+      </c>
+      <c r="R6" s="14" t="str">
+        <f>IFERROR(VLOOKUP(D6,[1]!SearchCT[#Data],2,FALSE),"")</f>
+        <v/>
+      </c>
+      <c r="S6" s="13" t="str">
+        <f>IFERROR(VLOOKUP(D6,[1]!SearchCT[#Data],3,FALSE),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="7" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A7" s="52" t="s">
+        <v>24</v>
+      </c>
+      <c r="D7" s="12" t="s">
+        <v>103</v>
+      </c>
+      <c r="E7" s="22" t="s">
+        <v>175</v>
+      </c>
+      <c r="F7" s="11" t="s">
+        <v>169</v>
+      </c>
+      <c r="H7" s="21" t="str">
+        <f>VLOOKUP(D7,[1]!Dictionary[#All],3,FALSE)</f>
+        <v>Artifact</v>
+      </c>
+      <c r="I7" s="20">
+        <f>VLOOKUP(D7,[1]!Dictionary[#All],4,FALSE)</f>
+        <v>11296</v>
+      </c>
+      <c r="J7" s="20" t="str">
+        <f>VLOOKUP(D7,[1]!Dictionary[#All],5,FALSE)</f>
+        <v>RADLEX</v>
+      </c>
+      <c r="K7" s="19">
+        <f>VLOOKUP(D7,[1]!Dictionary[#All],6,FALSE)</f>
+        <v>3.8</v>
+      </c>
+      <c r="L7" s="18" t="str">
+        <f>VLOOKUP(D7,[1]!VolumeType[#All],2,FALSE)</f>
+        <v>Artifact</v>
+      </c>
+      <c r="M7" s="17" t="str">
+        <f>VLOOKUP(D7,[1]!VolumeType[#All],3,FALSE)</f>
+        <v>None</v>
+      </c>
+      <c r="N7" s="16" t="str">
+        <f>VLOOKUP(D7,[1]!Colors[#All],3,FALSE)</f>
+        <v>z RO Helper</v>
+      </c>
+      <c r="O7" s="14" t="str">
+        <f>IFERROR(VLOOKUP(D7,[1]!DVH_lines[#Data],2,FALSE),"")</f>
+        <v/>
+      </c>
+      <c r="P7" s="15" t="str">
+        <f>IFERROR(VLOOKUP(D7,[1]!DVH_lines[#Data],3,FALSE),"")</f>
+        <v/>
+      </c>
+      <c r="Q7" s="13" t="str">
+        <f>IFERROR(VLOOKUP(D7,[1]!DVH_lines[#Data],4,FALSE),"")</f>
+        <v/>
+      </c>
+      <c r="R7" s="14" t="str">
+        <f>IFERROR(VLOOKUP(D7,[1]!SearchCT[#Data],2,FALSE),"")</f>
+        <v/>
+      </c>
+      <c r="S7" s="13" t="str">
+        <f>IFERROR(VLOOKUP(D7,[1]!SearchCT[#Data],3,FALSE),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="8" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A8" s="52" t="s">
+        <v>20</v>
+      </c>
+      <c r="B8" s="52" t="s">
+        <v>19</v>
+      </c>
+      <c r="D8" s="12" t="s">
+        <v>103</v>
+      </c>
+      <c r="E8" s="22" t="s">
+        <v>176</v>
+      </c>
+      <c r="F8" s="11" t="s">
+        <v>169</v>
+      </c>
+      <c r="H8" s="21" t="str">
+        <f>VLOOKUP(D8,[1]!Dictionary[#All],3,FALSE)</f>
+        <v>Artifact</v>
+      </c>
+      <c r="I8" s="20">
+        <f>VLOOKUP(D8,[1]!Dictionary[#All],4,FALSE)</f>
+        <v>11296</v>
+      </c>
+      <c r="J8" s="20" t="str">
+        <f>VLOOKUP(D8,[1]!Dictionary[#All],5,FALSE)</f>
+        <v>RADLEX</v>
+      </c>
+      <c r="K8" s="19">
+        <f>VLOOKUP(D8,[1]!Dictionary[#All],6,FALSE)</f>
+        <v>3.8</v>
+      </c>
+      <c r="L8" s="18" t="str">
+        <f>VLOOKUP(D8,[1]!VolumeType[#All],2,FALSE)</f>
+        <v>Artifact</v>
+      </c>
+      <c r="M8" s="17" t="str">
+        <f>VLOOKUP(D8,[1]!VolumeType[#All],3,FALSE)</f>
+        <v>None</v>
+      </c>
+      <c r="N8" s="16" t="str">
+        <f>VLOOKUP(D8,[1]!Colors[#All],3,FALSE)</f>
+        <v>z RO Helper</v>
+      </c>
+      <c r="O8" s="14" t="str">
+        <f>IFERROR(VLOOKUP(D8,[1]!DVH_lines[#Data],2,FALSE),"")</f>
+        <v/>
+      </c>
+      <c r="P8" s="15" t="str">
+        <f>IFERROR(VLOOKUP(D8,[1]!DVH_lines[#Data],3,FALSE),"")</f>
+        <v/>
+      </c>
+      <c r="Q8" s="13" t="str">
+        <f>IFERROR(VLOOKUP(D8,[1]!DVH_lines[#Data],4,FALSE),"")</f>
+        <v/>
+      </c>
+      <c r="R8" s="14" t="str">
+        <f>IFERROR(VLOOKUP(D8,[1]!SearchCT[#Data],2,FALSE),"")</f>
+        <v/>
+      </c>
+      <c r="S8" s="13" t="str">
+        <f>IFERROR(VLOOKUP(D8,[1]!SearchCT[#Data],3,FALSE),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="9" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A9" s="52" t="s">
+        <v>159</v>
+      </c>
+      <c r="B9" s="52" t="s">
+        <v>153</v>
+      </c>
+      <c r="D9" s="12" t="s">
+        <v>186</v>
+      </c>
+      <c r="E9" s="11" t="s">
+        <v>177</v>
+      </c>
+      <c r="F9" s="11" t="s">
+        <v>180</v>
+      </c>
+      <c r="H9" s="21" t="str">
+        <f>VLOOKUP(D9,[1]!Dictionary[#All],3,FALSE)</f>
+        <v>GTV Primary</v>
+      </c>
+      <c r="I9" s="20" t="str">
+        <f>VLOOKUP(D9,[1]!Dictionary[#All],4,FALSE)</f>
+        <v>GTVp</v>
+      </c>
+      <c r="J9" s="20" t="str">
+        <f>VLOOKUP(D9,[1]!Dictionary[#All],5,FALSE)</f>
+        <v>99VMS_STRUCTCODE</v>
+      </c>
+      <c r="K9" s="19" t="str">
+        <f>VLOOKUP(D9,[1]!Dictionary[#All],6,FALSE)</f>
+        <v>1.0</v>
+      </c>
+      <c r="L9" s="18" t="str">
+        <f>VLOOKUP(D9,[1]!VolumeType[#All],2,FALSE)</f>
+        <v>GTV</v>
+      </c>
+      <c r="M9" s="17" t="str">
+        <f>VLOOKUP(D9,[1]!VolumeType[#All],3,FALSE)</f>
+        <v>GTV</v>
+      </c>
+      <c r="N9" s="16" t="str">
+        <f>VLOOKUP(D9,[1]!Colors[#All],3,FALSE)</f>
+        <v>z GTV</v>
+      </c>
+      <c r="O9" s="14" t="str">
+        <f>IFERROR(VLOOKUP(D9,[1]!DVH_lines[#Data],2,FALSE),"")</f>
+        <v/>
+      </c>
+      <c r="P9" s="15" t="str">
+        <f>IFERROR(VLOOKUP(D9,[1]!DVH_lines[#Data],3,FALSE),"")</f>
+        <v/>
+      </c>
+      <c r="Q9" s="13" t="str">
+        <f>IFERROR(VLOOKUP(D9,[1]!DVH_lines[#Data],4,FALSE),"")</f>
+        <v/>
+      </c>
+      <c r="R9" s="14" t="str">
+        <f>IFERROR(VLOOKUP(D9,[1]!SearchCT[#Data],2,FALSE),"")</f>
+        <v/>
+      </c>
+      <c r="S9" s="13" t="str">
+        <f>IFERROR(VLOOKUP(D9,[1]!SearchCT[#Data],3,FALSE),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="10" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A10" s="52" t="s">
+        <v>150</v>
+      </c>
+      <c r="B10" s="52" t="s">
+        <v>151</v>
+      </c>
+      <c r="D10" s="12" t="s">
+        <v>185</v>
+      </c>
+      <c r="E10" s="11" t="s">
+        <v>178</v>
+      </c>
+      <c r="F10" s="11" t="s">
+        <v>181</v>
+      </c>
+      <c r="H10" s="21" t="str">
+        <f>VLOOKUP(D10,[1]!Dictionary[#All],3,FALSE)</f>
+        <v>CTV Primary</v>
+      </c>
+      <c r="I10" s="20" t="str">
+        <f>VLOOKUP(D10,[1]!Dictionary[#All],4,FALSE)</f>
+        <v>CTVp</v>
+      </c>
+      <c r="J10" s="20" t="str">
+        <f>VLOOKUP(D10,[1]!Dictionary[#All],5,FALSE)</f>
+        <v>99VMS_STRUCTCODE</v>
+      </c>
+      <c r="K10" s="19" t="str">
+        <f>VLOOKUP(D10,[1]!Dictionary[#All],6,FALSE)</f>
+        <v>1.0</v>
+      </c>
+      <c r="L10" s="18" t="str">
+        <f>VLOOKUP(D10,[1]!VolumeType[#All],2,FALSE)</f>
+        <v>CTV</v>
+      </c>
+      <c r="M10" s="17" t="str">
+        <f>VLOOKUP(D10,[1]!VolumeType[#All],3,FALSE)</f>
+        <v>CTV</v>
+      </c>
+      <c r="N10" s="16" t="str">
+        <f>VLOOKUP(D10,[1]!Colors[#All],3,FALSE)</f>
+        <v>z CTV</v>
+      </c>
+      <c r="O10" s="14" t="str">
+        <f>IFERROR(VLOOKUP(D10,[1]!DVH_lines[#Data],2,FALSE),"")</f>
+        <v/>
+      </c>
+      <c r="P10" s="15" t="str">
+        <f>IFERROR(VLOOKUP(D10,[1]!DVH_lines[#Data],3,FALSE),"")</f>
+        <v/>
+      </c>
+      <c r="Q10" s="13" t="str">
+        <f>IFERROR(VLOOKUP(D10,[1]!DVH_lines[#Data],4,FALSE),"")</f>
+        <v/>
+      </c>
+      <c r="R10" s="14" t="str">
+        <f>IFERROR(VLOOKUP(D10,[1]!SearchCT[#Data],2,FALSE),"")</f>
+        <v/>
+      </c>
+      <c r="S10" s="13" t="str">
+        <f>IFERROR(VLOOKUP(D10,[1]!SearchCT[#Data],3,FALSE),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="11" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="52" t="s">
+        <v>167</v>
+      </c>
+      <c r="B11" s="52" t="s">
+        <v>183</v>
+      </c>
+      <c r="D11" s="12" t="s">
+        <v>184</v>
+      </c>
+      <c r="E11" s="11" t="s">
+        <v>179</v>
+      </c>
+      <c r="F11" s="11" t="s">
+        <v>182</v>
+      </c>
+      <c r="H11" s="10" t="str">
+        <f>VLOOKUP(D11,[1]!Dictionary[#All],3,FALSE)</f>
+        <v>PTV Primary</v>
+      </c>
+      <c r="I11" s="9" t="str">
+        <f>VLOOKUP(D11,[1]!Dictionary[#All],4,FALSE)</f>
+        <v>PTVp</v>
+      </c>
+      <c r="J11" s="9" t="str">
+        <f>VLOOKUP(D11,[1]!Dictionary[#All],5,FALSE)</f>
+        <v>99VMS_STRUCTCODE</v>
+      </c>
+      <c r="K11" s="8" t="str">
+        <f>VLOOKUP(D11,[1]!Dictionary[#All],6,FALSE)</f>
+        <v>1.0</v>
+      </c>
+      <c r="L11" s="7" t="str">
+        <f>VLOOKUP(D11,[1]!VolumeType[#All],2,FALSE)</f>
+        <v>PTV</v>
+      </c>
+      <c r="M11" s="6" t="str">
+        <f>VLOOKUP(D11,[1]!VolumeType[#All],3,FALSE)</f>
+        <v>PTV</v>
+      </c>
+      <c r="N11" s="5" t="str">
+        <f>VLOOKUP(D11,[1]!Colors[#All],3,FALSE)</f>
+        <v>z PTV</v>
+      </c>
+      <c r="O11" s="3" t="str">
+        <f>IFERROR(VLOOKUP(D11,[1]!DVH_lines[#Data],2,FALSE),"")</f>
+        <v/>
+      </c>
+      <c r="P11" s="4" t="str">
+        <f>IFERROR(VLOOKUP(D11,[1]!DVH_lines[#Data],3,FALSE),"")</f>
+        <v/>
+      </c>
+      <c r="Q11" s="2" t="str">
+        <f>IFERROR(VLOOKUP(D11,[1]!DVH_lines[#Data],4,FALSE),"")</f>
+        <v/>
+      </c>
+      <c r="R11" s="3" t="str">
+        <f>IFERROR(VLOOKUP(D11,[1]!SearchCT[#Data],2,FALSE),"")</f>
+        <v/>
+      </c>
+      <c r="S11" s="2" t="str">
+        <f>IFERROR(VLOOKUP(D11,[1]!SearchCT[#Data],3,FALSE),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="12" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A12" s="52" t="s">
+        <v>152</v>
+      </c>
+      <c r="B12" s="52" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="13" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A13" s="52" t="s">
+        <v>12</v>
+      </c>
+      <c r="B13" s="52" t="s">
+        <v>11</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="6">
+    <mergeCell ref="R1:S1"/>
+    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="D1:F1"/>
+    <mergeCell ref="H1:K1"/>
+    <mergeCell ref="L1:M1"/>
+    <mergeCell ref="O1:Q1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup scale="93" orientation="landscape" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+  <tableParts count="2">
+    <tablePart r:id="rId2"/>
+    <tablePart r:id="rId3"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr>
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
+  <dimension ref="A1:S13"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
@@ -6672,7 +7713,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>

</xml_diff>

<commit_message>
SIB Templates Import Export Config
Added SIB templates
Updated RO Resident (X) template
Added Import/Export Template Config file
</commit_message>
<xml_diff>
--- a/External Beam Templates/Structure Templates/Template Spreadsheets/Specialty Templates.xlsx
+++ b/External Beam Templates/Structure Templates/Template Spreadsheets/Specialty Templates.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="518" uniqueCount="187">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="518" uniqueCount="188">
   <si>
     <t>Bolus X cm thickness</t>
   </si>
@@ -584,6 +584,9 @@
   </si>
   <si>
     <t>GTV</t>
+  </si>
+  <si>
+    <t>RO Resident</t>
   </si>
 </sst>
 </file>
@@ -2759,6 +2762,7 @@
       <sheetName val="ICD-10 Codes"/>
       <sheetName val="Color Chart"/>
       <sheetName val="Original Structure colors"/>
+      <sheetName val="ColourTable"/>
     </sheetNames>
     <sheetDataSet>
       <sheetData sheetId="0"/>
@@ -2772,6 +2776,7 @@
       <sheetData sheetId="8"/>
       <sheetData sheetId="9"/>
       <sheetData sheetId="10"/>
+      <sheetData sheetId="11"/>
     </sheetDataSet>
   </externalBook>
 </externalLink>
@@ -6405,7 +6410,7 @@
   <dimension ref="A1:S13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+      <selection activeCell="J7" sqref="J7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6529,7 +6534,7 @@
       </c>
       <c r="C3" s="24"/>
       <c r="D3" s="23" t="s">
-        <v>103</v>
+        <v>187</v>
       </c>
       <c r="E3" s="22" t="s">
         <v>171</v>
@@ -6563,7 +6568,7 @@
       </c>
       <c r="N3" s="16" t="str">
         <f>VLOOKUP(D3,[1]!Colors[#All],3,FALSE)</f>
-        <v>z RO Helper</v>
+        <v>Yellow</v>
       </c>
       <c r="O3" s="14" t="str">
         <f>IFERROR(VLOOKUP(D3,[1]!DVH_lines[#Data],2,FALSE),"")</f>
@@ -6595,7 +6600,7 @@
       </c>
       <c r="C4" s="24"/>
       <c r="D4" s="12" t="s">
-        <v>103</v>
+        <v>187</v>
       </c>
       <c r="E4" s="22" t="s">
         <v>172</v>
@@ -6629,7 +6634,7 @@
       </c>
       <c r="N4" s="16" t="str">
         <f>VLOOKUP(D4,[1]!Colors[#All],3,FALSE)</f>
-        <v>z RO Helper</v>
+        <v>Yellow</v>
       </c>
       <c r="O4" s="14" t="str">
         <f>IFERROR(VLOOKUP(D4,[1]!DVH_lines[#Data],2,FALSE),"")</f>
@@ -6661,7 +6666,7 @@
       </c>
       <c r="C5" s="24"/>
       <c r="D5" s="12" t="s">
-        <v>103</v>
+        <v>187</v>
       </c>
       <c r="E5" s="22" t="s">
         <v>173</v>
@@ -6695,7 +6700,7 @@
       </c>
       <c r="N5" s="16" t="str">
         <f>VLOOKUP(D5,[1]!Colors[#All],3,FALSE)</f>
-        <v>z RO Helper</v>
+        <v>Yellow</v>
       </c>
       <c r="O5" s="14" t="str">
         <f>IFERROR(VLOOKUP(D5,[1]!DVH_lines[#Data],2,FALSE),"")</f>
@@ -6727,7 +6732,7 @@
       </c>
       <c r="C6" s="24"/>
       <c r="D6" s="12" t="s">
-        <v>103</v>
+        <v>187</v>
       </c>
       <c r="E6" s="22" t="s">
         <v>174</v>
@@ -6761,7 +6766,7 @@
       </c>
       <c r="N6" s="16" t="str">
         <f>VLOOKUP(D6,[1]!Colors[#All],3,FALSE)</f>
-        <v>z RO Helper</v>
+        <v>Yellow</v>
       </c>
       <c r="O6" s="14" t="str">
         <f>IFERROR(VLOOKUP(D6,[1]!DVH_lines[#Data],2,FALSE),"")</f>
@@ -6789,7 +6794,7 @@
         <v>24</v>
       </c>
       <c r="D7" s="12" t="s">
-        <v>103</v>
+        <v>187</v>
       </c>
       <c r="E7" s="22" t="s">
         <v>175</v>
@@ -6823,7 +6828,7 @@
       </c>
       <c r="N7" s="16" t="str">
         <f>VLOOKUP(D7,[1]!Colors[#All],3,FALSE)</f>
-        <v>z RO Helper</v>
+        <v>Yellow</v>
       </c>
       <c r="O7" s="14" t="str">
         <f>IFERROR(VLOOKUP(D7,[1]!DVH_lines[#Data],2,FALSE),"")</f>
@@ -6854,7 +6859,7 @@
         <v>19</v>
       </c>
       <c r="D8" s="12" t="s">
-        <v>103</v>
+        <v>187</v>
       </c>
       <c r="E8" s="22" t="s">
         <v>176</v>
@@ -6888,7 +6893,7 @@
       </c>
       <c r="N8" s="16" t="str">
         <f>VLOOKUP(D8,[1]!Colors[#All],3,FALSE)</f>
-        <v>z RO Helper</v>
+        <v>Yellow</v>
       </c>
       <c r="O8" s="14" t="str">
         <f>IFERROR(VLOOKUP(D8,[1]!DVH_lines[#Data],2,FALSE),"")</f>

</xml_diff>